<commit_message>
Add doughnutchart in home
</commit_message>
<xml_diff>
--- a/data/fake_data.xlsx
+++ b/data/fake_data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F52D7B-563E-45DD-B080-80D3F57617E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,6 +281,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -315,6 +333,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,20 +525,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -555,7 +590,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -581,7 +616,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -607,7 +642,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -633,7 +668,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -656,10 +691,10 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -685,7 +720,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -708,10 +743,10 @@
         <v>15</v>
       </c>
       <c r="H8">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -734,10 +769,10 @@
         <v>15</v>
       </c>
       <c r="H9">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -760,10 +795,10 @@
         <v>10</v>
       </c>
       <c r="H10">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -786,10 +821,10 @@
         <v>10</v>
       </c>
       <c r="H11">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -812,10 +847,10 @@
         <v>11</v>
       </c>
       <c r="H12">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -838,10 +873,10 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -864,7 +899,7 @@
         <v>15</v>
       </c>
       <c r="H14">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>